<commit_message>
completed school_attendance model and view, completed report card model
</commit_message>
<xml_diff>
--- a/tests/static/Report_Card_Test_Data.xlsx
+++ b/tests/static/Report_Card_Test_Data.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="95">
   <si>
     <t>LOCAL ID</t>
   </si>
@@ -312,6 +312,9 @@
   </si>
   <si>
     <t>MarkelID</t>
+  </si>
+  <si>
+    <t>Jib Jabbin</t>
   </si>
 </sst>
 </file>
@@ -696,10 +699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CG11"/>
+  <dimension ref="A1:CG25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="U8" sqref="U8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1474,7 +1477,10 @@
         <v>0</v>
       </c>
       <c r="W7" s="6">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="X7" s="6" t="s">
+        <v>94</v>
       </c>
       <c r="AC7" s="6" t="s">
         <v>62</v>
@@ -1892,7 +1898,32 @@
         <v>92</v>
       </c>
     </row>
+    <row r="20" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="P20" s="1"/>
+    </row>
+    <row r="21" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="P21" s="1"/>
+    </row>
+    <row r="22" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="P22" s="1"/>
+    </row>
+    <row r="23" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="P23" s="1"/>
+    </row>
+    <row r="24" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="P24" s="1"/>
+    </row>
+    <row r="25" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="P25" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>